<commit_message>
Update docs + Burn down Chart
</commit_message>
<xml_diff>
--- a/Documenten/backlog.xlsx
+++ b/Documenten/backlog.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Molenaers\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project\IctProjectIBeaconsLaravel\Documenten\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21525" windowHeight="5820"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21525" windowHeight="5820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t xml:space="preserve">Als gebruiker wil ik dat de app statische info toont zodra ik me in de range van een beacon bevindt. </t>
   </si>
@@ -84,13 +84,26 @@
   </si>
   <si>
     <t>Als beheerder moet ik kunnen inloggen met de juiste gegevens om toegang te krijgen tot de webapp.</t>
+  </si>
+  <si>
+    <t>Tekst</t>
+  </si>
+  <si>
+    <t>Totaal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,19 +132,117 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -142,6 +253,19 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{2292557A-9E4D-4ED9-BED5-731746C200A5}" name="Tabel4" displayName="Tabel4" ref="C2:F19" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="C2:F19" xr:uid="{C006EA97-1BB0-4D9B-BBEE-430FEE91A7A3}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{4C4DA5B2-ADAE-4265-8FAA-F5014308C29E}" name="Volgorde" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{22C6F746-50F0-4E07-A045-03317E7EE93F}" name="Tekst" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{F6EB7528-F31A-4655-8FB2-5BA912AE26CC}" name="value" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{AE136A8C-A04C-4B7F-828A-C4FFE616C429}" name="Opmerkingen" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -406,24 +530,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:F20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="C2:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="174.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9.140625" style="2"/>
+    <col min="3" max="3" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="174.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D2" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="E2" s="1" t="s">
         <v>1</v>
       </c>
@@ -432,10 +562,10 @@
       </c>
     </row>
     <row r="3" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C3" s="2">
+      <c r="C3" s="3">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E3" s="1">
@@ -443,10 +573,10 @@
       </c>
     </row>
     <row r="4" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C4" s="2">
+      <c r="C4" s="3">
         <v>2</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E4" s="1">
@@ -454,10 +584,10 @@
       </c>
     </row>
     <row r="5" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C5" s="2">
+      <c r="C5" s="3">
         <v>3</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E5" s="1">
@@ -465,10 +595,10 @@
       </c>
     </row>
     <row r="6" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C6" s="2">
+      <c r="C6" s="3">
         <v>4</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E6" s="1">
@@ -476,10 +606,10 @@
       </c>
     </row>
     <row r="7" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C7" s="2">
+      <c r="C7" s="3">
         <v>5</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="1">
@@ -487,10 +617,10 @@
       </c>
     </row>
     <row r="8" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C8" s="2">
+      <c r="C8" s="3">
         <v>6</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E8" s="1">
@@ -498,24 +628,24 @@
       </c>
     </row>
     <row r="9" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C9" s="2">
+      <c r="C9" s="3">
         <v>7</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E9" s="1">
         <v>2</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C10" s="2">
+      <c r="C10" s="3">
         <v>8</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E10" s="1">
@@ -523,10 +653,10 @@
       </c>
     </row>
     <row r="11" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C11" s="2">
+      <c r="C11" s="3">
         <v>9</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E11" s="1">
@@ -534,10 +664,10 @@
       </c>
     </row>
     <row r="12" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C12" s="2">
+      <c r="C12" s="3">
         <v>10</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E12" s="1">
@@ -545,10 +675,10 @@
       </c>
     </row>
     <row r="13" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C13" s="2">
+      <c r="C13" s="3">
         <v>11</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E13" s="1">
@@ -556,10 +686,10 @@
       </c>
     </row>
     <row r="14" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C14" s="2">
+      <c r="C14" s="3">
         <v>12</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E14" s="1">
@@ -567,10 +697,10 @@
       </c>
     </row>
     <row r="15" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C15" s="2">
+      <c r="C15" s="3">
         <v>13</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E15" s="1">
@@ -578,10 +708,10 @@
       </c>
     </row>
     <row r="16" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C16" s="2">
+      <c r="C16" s="3">
         <v>14</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E16" s="1">
@@ -589,10 +719,10 @@
       </c>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C17" s="2">
+      <c r="C17" s="3">
         <v>15</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E17" s="1">
@@ -600,18 +730,21 @@
       </c>
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C18" s="2">
+      <c r="C18" s="3">
         <v>16</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E18" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="E20">
+    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D19" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="4">
         <f>SUM(E3:E18)</f>
         <v>71</v>
       </c>
@@ -619,5 +752,8 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>